<commit_message>
Add option to load from both
</commit_message>
<xml_diff>
--- a/Exp_Record_Alfa.xlsx
+++ b/Exp_Record_Alfa.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7182B159-017F-4AE1-B577-C33331AA62D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="373">
   <si>
     <t>Exp_collection</t>
   </si>
@@ -643,6 +637,79 @@
 40 mins 16 blocks</t>
   </si>
   <si>
+    <t>001 Rf mapping start at 14:34
+-8:2:8 2deg</t>
+  </si>
+  <si>
+    <t>003 RF mapping starts 14:45
+-1.5:0.75:1.5  0.75 deg</t>
+  </si>
+  <si>
+    <t>004 Generate Integrated 14:54
+Testing if we don't use baseline subtracted score, can we evolve faster.
+12 [-0.5 -0.8] 1  3 deg
+30 gens
+Finish in 16 mins  plateau around 16 gens! Grows super fast!
+Very successful!</t>
+  </si>
+  <si>
+    <t>005 Generate integrated 15:14
+12 [-0.5 -0.8] 1  3 deg   ZOHA_Sphere_lr_euclid
+Mu exponential decay from 50 deg to 7.33deg in 100 generations, learning rate 1.5
+Try out my new optimizer!
+Optimizer found gradient around 16-18 gens , grow featues to excite the plateau part of the image.
+Exploration get down to 32 deg at gen 24.
+Seems to surpass the performance of CMAES finally!</t>
+  </si>
+  <si>
+    <t>006 Generate integrated 15:40
+12 [-0.5 -0.8] 1  3 deg   ZOHA_Sphere_lr_euclid
+Mu exponential decay from 50 deg to 20 deg in 100 generations, learning rate 1.5
+See if larger exploration will result in different evolutions trajectory?
+Want to test if I decayed the learning rate too fast or too slow, because both could result in a slow optimization.
+See which part of the experiment does the firing rate grows the fastest! May be that is the right rate to go.
+Starts growing around gen 16-18, exploration = 41.5. At gen 23 the step between basis are 0.442.
+Close to 30 gens, still around 38.9 degree exploration.
+Seems the plateau around 150ms doesn't evolve successfully
+Starts growing the plateau around 32 gens.
+Obviously, the evolution is much less smooth than the last one! Many stagnant and coming in and out.
+Around 35 gens still 36.5 degrees.
+37 gens 35.8 degree,
+This is much slower than the 2nd, ZOHA Sphere_lr_euclide, and slower than the first CMA-ES,
+PSTH seems different from the last one, the gap between the 2 peaks are longer!
+At around 50 gens reached 450 just
+This schedule seems not very helpful……. Try others</t>
+  </si>
+  <si>
+    <t>007 Generate Integrated 16:12
+12 [-0.5 -0.8] 1  3 deg   ZOHA_Sphere_lr_euclid
+Mu exponential decay from 40 deg to 10 deg in 100 generations, learning rate 1.5
+See if smaller exploration will result in better evolutions trajectory?
+At gen 9, the exploration around 35.3 deg
+Speed of this optimizer is similar to CMAES! Grows super fast, Exploration range around 32.9 at 15gens.
+Perhaps exploration range around 30-35deg is the sweet spot?
+Reach 400 around 30 gens, similar PSTH.
+Faster than the last one. But curiously, the result doesn't look as</t>
+  </si>
+  <si>
+    <t>008 Generate Integrated 16:45
+64 [0 -2.1] 1  4deg  ZOHA_Sphere_lr_euclid
+Same learning rate scheduling with last experiment,
+Mu exponential decay from 40 deg to 10 deg in 100 generations, learning rate 1.5
+The firing rate PSTH is very sustained! Like square wave.
+Starts growing steadily from 5 gens.
+Grow not very fast. Starts to plateau around 20 gens.
+But the learning rate schedule tuned for</t>
+  </si>
+  <si>
+    <t>009 Generate Integrated 17:03
+64 [0 -2.1]  1 4deg  ZOHA_Sphere_lr_euclid
+Mu exponential decay from 40 deg to 5 deg in 100 generations, learning rate 1.5
+Faster decay to small learning rate, see how it goes!
+The result doesn't change significantly! Seems similar speed and result
+He is a very good boy today! Seems he can give me 20 gens for this</t>
+  </si>
+  <si>
     <t>Alfa64chan-19112019-009</t>
   </si>
   <si>
@@ -898,6 +965,30 @@
     <t>Alfa64chan-10032020-006</t>
   </si>
   <si>
+    <t>Alfa64chan-16032020-001</t>
+  </si>
+  <si>
+    <t>Alfa64chan-16032020-003</t>
+  </si>
+  <si>
+    <t>Alfa64chan-16032020-004</t>
+  </si>
+  <si>
+    <t>Alfa64chan-16032020-005</t>
+  </si>
+  <si>
+    <t>Alfa64chan-16032020-006</t>
+  </si>
+  <si>
+    <t>Alfa64chan-16032020-007</t>
+  </si>
+  <si>
+    <t>Alfa64chan-16032020-008</t>
+  </si>
+  <si>
+    <t>Alfa64chan-16032020-009</t>
+  </si>
+  <si>
     <t>191119_Alfa_generate_parallel(3)</t>
   </si>
   <si>
@@ -1153,6 +1244,30 @@
     <t>200310_Alfa_generate_integrated(4)</t>
   </si>
   <si>
+    <t>200316_Alfa_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200316_Alfa_rfMapper_basic(2)</t>
+  </si>
+  <si>
+    <t>200316_Alfa_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200316_Alfa_generate_integrated(2)</t>
+  </si>
+  <si>
+    <t>200316_Alfa_generate_integrated(3)</t>
+  </si>
+  <si>
+    <t>200316_Alfa_generate_integrated(4)</t>
+  </si>
+  <si>
+    <t>200316_Alfa_generate_integrated(5)</t>
+  </si>
+  <si>
+    <t>200316_Alfa_generate_integrated(6)</t>
+  </si>
+  <si>
     <t>N:\Stimuli\2019-06-Evolutions\alfa-191119a</t>
   </si>
   <si>
@@ -1382,13 +1497,34 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-12-Evolutions\2020-03-10-Alfa-04\2020-03-10-15-29-12</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-06-RF-mapping\2020-03-16-Alfa</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-16-Alfa-01\2020-03-16-14-54-33</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-16-Alfa-02\2020-03-16-15-14-25</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-16-Alfa-03\2020-03-16-15-40-58</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-16-Alfa-04\2020-03-16-16-12-37</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-16-Alfa-05\2020-03-16-16-45-43</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-12-Evolutions\2020-03-16-Alfa-06\2020-03-16-17-03-32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1447,23 +1583,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1505,7 +1633,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1537,27 +1665,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1589,24 +1699,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1782,21 +1874,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="95.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1822,7 +1907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1833,10 +1918,10 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="F2">
         <v>29</v>
@@ -1845,10 +1930,10 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1859,10 +1944,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="F3">
         <v>29</v>
@@ -1871,7 +1956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1882,10 +1967,10 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="F4">
         <v>29</v>
@@ -1894,10 +1979,10 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1908,10 +1993,10 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="F5">
         <v>29</v>
@@ -1920,10 +2005,10 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1934,19 +2019,19 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="F6">
         <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1957,10 +2042,10 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="F7">
         <v>29</v>
@@ -1969,10 +2054,10 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1983,10 +2068,10 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="F8">
         <v>9</v>
@@ -1995,10 +2080,10 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2009,10 +2094,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="F9">
         <v>9</v>
@@ -2021,10 +2106,10 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2035,10 +2120,10 @@
         <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E10" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -2047,10 +2132,10 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -2061,10 +2146,10 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E11" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="F11">
         <v>32</v>
@@ -2073,10 +2158,10 @@
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2087,10 +2172,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="F12">
         <v>32</v>
@@ -2099,10 +2184,10 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2113,10 +2198,10 @@
         <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="F13">
         <v>32</v>
@@ -2125,21 +2210,21 @@
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="C14" t="s">
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E14" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2150,10 +2235,10 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="E15" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -2162,10 +2247,10 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -2176,10 +2261,10 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E16" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -2188,10 +2273,10 @@
         <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -2202,10 +2287,10 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E17" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -2214,21 +2299,21 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="C18" t="s">
         <v>26</v>
       </c>
       <c r="D18" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2239,10 +2324,10 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="E19" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="F19">
         <v>7</v>
@@ -2251,10 +2336,10 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2265,10 +2350,10 @@
         <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="F20">
         <v>7</v>
@@ -2277,10 +2362,10 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2291,10 +2376,10 @@
         <v>29</v>
       </c>
       <c r="D21" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E21" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="F21">
         <v>7</v>
@@ -2303,66 +2388,66 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="C22" t="s">
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="C23" t="s">
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="E23" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="C24" t="s">
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="G24">
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="C25" t="s">
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -2373,10 +2458,10 @@
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="E26" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="F26">
         <v>51</v>
@@ -2385,10 +2470,10 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -2399,10 +2484,10 @@
         <v>35</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E27" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="F27">
         <v>51</v>
@@ -2411,10 +2496,10 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -2425,10 +2510,10 @@
         <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="E28" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="F28">
         <v>51</v>
@@ -2437,21 +2522,21 @@
         <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="C29" t="s">
         <v>37</v>
       </c>
       <c r="D29" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="E29" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -2462,10 +2547,10 @@
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="E30" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="F30">
         <v>7</v>
@@ -2474,10 +2559,10 @@
         <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -2488,10 +2573,10 @@
         <v>39</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="E31" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="F31">
         <v>7</v>
@@ -2500,10 +2585,10 @@
         <v>3</v>
       </c>
       <c r="H31" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2514,10 +2599,10 @@
         <v>40</v>
       </c>
       <c r="D32" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E32" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="F32">
         <v>7</v>
@@ -2526,21 +2611,21 @@
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="C33" t="s">
         <v>41</v>
       </c>
       <c r="D33" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E33" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -2551,10 +2636,10 @@
         <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="F34">
         <v>7</v>
@@ -2563,10 +2648,10 @@
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -2577,10 +2662,10 @@
         <v>43</v>
       </c>
       <c r="D35" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E35" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="F35">
         <v>7</v>
@@ -2589,10 +2674,10 @@
         <v>3</v>
       </c>
       <c r="H35" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2603,10 +2688,10 @@
         <v>44</v>
       </c>
       <c r="D36" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E36" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="F36">
         <v>7</v>
@@ -2615,10 +2700,10 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>8</v>
       </c>
@@ -2629,10 +2714,10 @@
         <v>45</v>
       </c>
       <c r="D37" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E37" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="F37">
         <v>36</v>
@@ -2641,10 +2726,10 @@
         <v>3</v>
       </c>
       <c r="H37" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2655,10 +2740,10 @@
         <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="E38" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="F38">
         <v>36</v>
@@ -2667,10 +2752,10 @@
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>8</v>
       </c>
@@ -2681,10 +2766,10 @@
         <v>47</v>
       </c>
       <c r="D39" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E39" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="F39">
         <v>35</v>
@@ -2693,10 +2778,10 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2707,10 +2792,10 @@
         <v>48</v>
       </c>
       <c r="D40" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E40" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="F40">
         <v>35</v>
@@ -2719,10 +2804,10 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>8</v>
       </c>
@@ -2733,10 +2818,10 @@
         <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E41" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="F41">
         <v>35</v>
@@ -2745,10 +2830,10 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2759,10 +2844,10 @@
         <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E42" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="F42">
         <v>61</v>
@@ -2771,10 +2856,10 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2785,10 +2870,10 @@
         <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E43" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="F43">
         <v>61</v>
@@ -2797,10 +2882,10 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>8</v>
       </c>
@@ -2811,10 +2896,10 @@
         <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E44" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="F44">
         <v>61</v>
@@ -2823,10 +2908,10 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -2837,10 +2922,10 @@
         <v>53</v>
       </c>
       <c r="D45" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E45" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
       <c r="F45">
         <v>33</v>
@@ -2849,10 +2934,10 @@
         <v>3</v>
       </c>
       <c r="H45" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>8</v>
       </c>
@@ -2863,10 +2948,10 @@
         <v>54</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E46" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="F46">
         <v>33</v>
@@ -2875,10 +2960,10 @@
         <v>3</v>
       </c>
       <c r="H46" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>8</v>
       </c>
@@ -2889,10 +2974,10 @@
         <v>55</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="E47" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
       <c r="F47">
         <v>33</v>
@@ -2901,10 +2986,10 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>8</v>
       </c>
@@ -2915,10 +3000,10 @@
         <v>56</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E48" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
       <c r="F48">
         <v>43</v>
@@ -2927,10 +3012,10 @@
         <v>3</v>
       </c>
       <c r="H48" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>8</v>
       </c>
@@ -2941,10 +3026,10 @@
         <v>57</v>
       </c>
       <c r="D49" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="E49" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="F49">
         <v>43</v>
@@ -2953,10 +3038,10 @@
         <v>3</v>
       </c>
       <c r="H49" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>8</v>
       </c>
@@ -2967,10 +3052,10 @@
         <v>58</v>
       </c>
       <c r="D50" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E50" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
       <c r="F50">
         <v>43</v>
@@ -2979,10 +3064,10 @@
         <v>3</v>
       </c>
       <c r="H50" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -2993,10 +3078,10 @@
         <v>59</v>
       </c>
       <c r="D51" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="E51" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
       <c r="F51">
         <v>59</v>
@@ -3005,10 +3090,10 @@
         <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -3019,10 +3104,10 @@
         <v>60</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="E52" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="F52">
         <v>59</v>
@@ -3031,10 +3116,10 @@
         <v>3</v>
       </c>
       <c r="H52" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -3045,10 +3130,10 @@
         <v>61</v>
       </c>
       <c r="D53" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E53" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="F53">
         <v>59</v>
@@ -3057,10 +3142,10 @@
         <v>3</v>
       </c>
       <c r="H53" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -3071,10 +3156,10 @@
         <v>62</v>
       </c>
       <c r="D54" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="E54" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="F54">
         <v>20</v>
@@ -3083,10 +3168,10 @@
         <v>3</v>
       </c>
       <c r="H54" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -3097,10 +3182,10 @@
         <v>63</v>
       </c>
       <c r="D55" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E55" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="F55">
         <v>20</v>
@@ -3109,10 +3194,10 @@
         <v>3</v>
       </c>
       <c r="H55" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>8</v>
       </c>
@@ -3123,10 +3208,10 @@
         <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="E56" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="F56">
         <v>20</v>
@@ -3135,10 +3220,10 @@
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>8</v>
       </c>
@@ -3149,10 +3234,10 @@
         <v>65</v>
       </c>
       <c r="D57" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E57" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="F57">
         <v>49</v>
@@ -3161,10 +3246,10 @@
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -3175,10 +3260,10 @@
         <v>66</v>
       </c>
       <c r="D58" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="E58" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
       <c r="F58">
         <v>49</v>
@@ -3187,10 +3272,10 @@
         <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -3201,10 +3286,10 @@
         <v>67</v>
       </c>
       <c r="D59" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E59" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="F59">
         <v>49</v>
@@ -3213,10 +3298,10 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>8</v>
       </c>
@@ -3227,10 +3312,10 @@
         <v>68</v>
       </c>
       <c r="D60" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="E60" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="F60">
         <v>19</v>
@@ -3239,10 +3324,10 @@
         <v>3</v>
       </c>
       <c r="H60" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>8</v>
       </c>
@@ -3253,10 +3338,10 @@
         <v>69</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="E61" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="F61">
         <v>19</v>
@@ -3265,10 +3350,10 @@
         <v>3</v>
       </c>
       <c r="H61" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -3279,10 +3364,10 @@
         <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="E62" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="F62">
         <v>19</v>
@@ -3291,10 +3376,10 @@
         <v>3</v>
       </c>
       <c r="H62" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>8</v>
       </c>
@@ -3305,10 +3390,10 @@
         <v>71</v>
       </c>
       <c r="D63" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E63" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="F63">
         <v>12</v>
@@ -3317,10 +3402,10 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>8</v>
       </c>
@@ -3331,10 +3416,10 @@
         <v>72</v>
       </c>
       <c r="D64" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E64" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="F64">
         <v>12</v>
@@ -3343,10 +3428,10 @@
         <v>3</v>
       </c>
       <c r="H64" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" t="s">
         <v>8</v>
       </c>
@@ -3357,10 +3442,10 @@
         <v>73</v>
       </c>
       <c r="D65" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="E65" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
       <c r="F65">
         <v>12</v>
@@ -3369,10 +3454,10 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -3383,10 +3468,10 @@
         <v>74</v>
       </c>
       <c r="D66" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="E66" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="F66">
         <v>41</v>
@@ -3395,10 +3480,10 @@
         <v>3</v>
       </c>
       <c r="H66" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" t="s">
         <v>8</v>
       </c>
@@ -3409,10 +3494,10 @@
         <v>75</v>
       </c>
       <c r="D67" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E67" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="F67">
         <v>41</v>
@@ -3421,10 +3506,10 @@
         <v>3</v>
       </c>
       <c r="H67" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" t="s">
         <v>8</v>
       </c>
@@ -3435,10 +3520,10 @@
         <v>76</v>
       </c>
       <c r="D68" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E68" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
       <c r="F68">
         <v>41</v>
@@ -3447,10 +3532,10 @@
         <v>3</v>
       </c>
       <c r="H68" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -3461,10 +3546,10 @@
         <v>77</v>
       </c>
       <c r="D69" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E69" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="F69">
         <v>63</v>
@@ -3473,10 +3558,10 @@
         <v>3</v>
       </c>
       <c r="H69" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -3487,10 +3572,10 @@
         <v>78</v>
       </c>
       <c r="D70" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E70" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="F70">
         <v>63</v>
@@ -3499,10 +3584,10 @@
         <v>3</v>
       </c>
       <c r="H70" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" t="s">
         <v>8</v>
       </c>
@@ -3513,10 +3598,10 @@
         <v>79</v>
       </c>
       <c r="D71" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="E71" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="F71">
         <v>63</v>
@@ -3525,10 +3610,10 @@
         <v>3</v>
       </c>
       <c r="H71" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
       <c r="A72" t="s">
         <v>8</v>
       </c>
@@ -3539,10 +3624,10 @@
         <v>80</v>
       </c>
       <c r="D72" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="E72" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="F72">
         <v>38</v>
@@ -3551,10 +3636,10 @@
         <v>3</v>
       </c>
       <c r="H72" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
       <c r="A73" t="s">
         <v>8</v>
       </c>
@@ -3565,10 +3650,10 @@
         <v>81</v>
       </c>
       <c r="D73" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="E73" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="F73">
         <v>38</v>
@@ -3577,10 +3662,10 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -3591,10 +3676,10 @@
         <v>82</v>
       </c>
       <c r="D74" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="E74" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="F74">
         <v>38</v>
@@ -3603,10 +3688,10 @@
         <v>3</v>
       </c>
       <c r="H74" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -3617,10 +3702,10 @@
         <v>83</v>
       </c>
       <c r="D75" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E75" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="F75">
         <v>39</v>
@@ -3629,10 +3714,10 @@
         <v>3</v>
       </c>
       <c r="H75" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -3643,10 +3728,10 @@
         <v>84</v>
       </c>
       <c r="D76" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E76" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="F76">
         <v>39</v>
@@ -3655,10 +3740,10 @@
         <v>3</v>
       </c>
       <c r="H76" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8">
       <c r="A77" t="s">
         <v>8</v>
       </c>
@@ -3669,10 +3754,10 @@
         <v>85</v>
       </c>
       <c r="D77" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="E77" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="F77">
         <v>39</v>
@@ -3681,10 +3766,10 @@
         <v>3</v>
       </c>
       <c r="H77" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8">
       <c r="A78" t="s">
         <v>8</v>
       </c>
@@ -3695,10 +3780,10 @@
         <v>86</v>
       </c>
       <c r="D78" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E78" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="F78">
         <v>44</v>
@@ -3707,10 +3792,10 @@
         <v>3</v>
       </c>
       <c r="H78" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8">
       <c r="A79" t="s">
         <v>8</v>
       </c>
@@ -3721,10 +3806,10 @@
         <v>87</v>
       </c>
       <c r="D79" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E79" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="F79">
         <v>44</v>
@@ -3733,10 +3818,10 @@
         <v>3</v>
       </c>
       <c r="H79" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
       <c r="A80" t="s">
         <v>8</v>
       </c>
@@ -3747,10 +3832,10 @@
         <v>88</v>
       </c>
       <c r="D80" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="E80" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
       <c r="F80">
         <v>44</v>
@@ -3759,10 +3844,10 @@
         <v>3</v>
       </c>
       <c r="H80" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -3770,16 +3855,16 @@
         <v>89</v>
       </c>
       <c r="D81" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E81" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="H81" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>9</v>
       </c>
@@ -3787,16 +3872,16 @@
         <v>90</v>
       </c>
       <c r="D82" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="E82" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="H82" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -3807,10 +3892,10 @@
         <v>91</v>
       </c>
       <c r="D83" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E83" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="F83">
         <v>13</v>
@@ -3819,10 +3904,10 @@
         <v>3</v>
       </c>
       <c r="H83" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>9</v>
       </c>
@@ -3833,10 +3918,10 @@
         <v>92</v>
       </c>
       <c r="D84" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="E84" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="F84">
         <v>28</v>
@@ -3845,10 +3930,10 @@
         <v>3</v>
       </c>
       <c r="H84" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>9</v>
       </c>
@@ -3859,10 +3944,10 @@
         <v>93</v>
       </c>
       <c r="D85" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="E85" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="F85">
         <v>20</v>
@@ -3871,10 +3956,10 @@
         <v>5</v>
       </c>
       <c r="H85" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>9</v>
       </c>
@@ -3885,10 +3970,10 @@
         <v>94</v>
       </c>
       <c r="D86" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E86" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="F86">
         <v>48</v>
@@ -3897,7 +3982,143 @@
         <v>3</v>
       </c>
       <c r="H86" t="s">
-        <v>341</v>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" t="s">
+        <v>188</v>
+      </c>
+      <c r="E87" t="s">
+        <v>281</v>
+      </c>
+      <c r="H87" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>96</v>
+      </c>
+      <c r="D88" t="s">
+        <v>189</v>
+      </c>
+      <c r="E88" t="s">
+        <v>282</v>
+      </c>
+      <c r="H88" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" t="s">
+        <v>97</v>
+      </c>
+      <c r="D89" t="s">
+        <v>190</v>
+      </c>
+      <c r="E89" t="s">
+        <v>283</v>
+      </c>
+      <c r="H89" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" t="s">
+        <v>98</v>
+      </c>
+      <c r="D90" t="s">
+        <v>191</v>
+      </c>
+      <c r="E90" t="s">
+        <v>284</v>
+      </c>
+      <c r="H90" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" t="s">
+        <v>99</v>
+      </c>
+      <c r="D91" t="s">
+        <v>192</v>
+      </c>
+      <c r="E91" t="s">
+        <v>285</v>
+      </c>
+      <c r="H91" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>100</v>
+      </c>
+      <c r="D92" t="s">
+        <v>193</v>
+      </c>
+      <c r="E92" t="s">
+        <v>286</v>
+      </c>
+      <c r="H92" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8">
+      <c r="A93" t="s">
+        <v>9</v>
+      </c>
+      <c r="C93" t="s">
+        <v>101</v>
+      </c>
+      <c r="D93" t="s">
+        <v>194</v>
+      </c>
+      <c r="E93" t="s">
+        <v>287</v>
+      </c>
+      <c r="H93" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" t="s">
+        <v>9</v>
+      </c>
+      <c r="C94" t="s">
+        <v>102</v>
+      </c>
+      <c r="D94" t="s">
+        <v>195</v>
+      </c>
+      <c r="E94" t="s">
+        <v>288</v>
+      </c>
+      <c r="H94" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add code fix append to collection
</commit_message>
<xml_diff>
--- a/Exp_Record_Alfa.xlsx
+++ b/Exp_Record_Alfa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18BB745-5BC8-4E78-A25B-7AA2FB94DBE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E55E34E-3142-4C52-91EF-8C5C62F28BBA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="1905" windowWidth="26295" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="1560" windowWidth="26295" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="887">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="914">
   <si>
     <t>Exp_collection</t>
   </si>
@@ -1728,6 +1728,58 @@
 4 blocks completed at 1158</t>
   </si>
   <si>
+    <t>Hp at around 1010
+001 at 1020 AM, rf mapping, 1, 3, 8 deg
+completed</t>
+  </si>
+  <si>
+    <t>Going for 54
+generate_integrated
+002 at 1032 AM
+54 (0,-0.5) 3 1 CMAES
+lasted around 16 minutes
+completed</t>
+  </si>
+  <si>
+    <t>003 at 1049 AM
+selectivity/manifold
+54 (0,-0.5) 3
+pasupathy refs
+86% performance at 1104, 3 blocks completed so far
+4 blocks as of 1108, 20 minutes…
+finished at 1112 AM, 5 reps
+completed</t>
+  </si>
+  <si>
+    <t>004 at 1113 AM
+57 (0,-0.5) 2 1 CMAES
+finished at 27 blocks
+completed</t>
+  </si>
+  <si>
+    <t>005 at 1126 AM
+57 ( 0 , -0.5) 2 selectivity/manifold
+4 reps at 1148 am
+completed
+completed</t>
+  </si>
+  <si>
+    <t>Last try, another evolution with IT. May or may not pan out.
+006 at 1149 AM
+generate integrated
+22 (-0.7,-2) 3 CMAES, 5/5 hash. Moderately good PSTH
+climbed to ~180 y gen 24, then jumped to 200 by gen 26.
+completed</t>
+  </si>
+  <si>
+    <t>007 at 1208 PM
+selectivity - manifold
+22 (-0.7,-2) 3, including pasupathy refs
+starting to blast at 130 ms; has had ~220 so far
+finishing at 4 reps at
+completed</t>
+  </si>
+  <si>
     <t>Alfa64chan-19112019-009</t>
   </si>
   <si>
@@ -2424,6 +2476,27 @@
     <t>Alfa64chan-28042020-007</t>
   </si>
   <si>
+    <t>Alfa64chan-29042020-001</t>
+  </si>
+  <si>
+    <t>Alfa64chan-29042020-002</t>
+  </si>
+  <si>
+    <t>Alfa64chan-29042020-003</t>
+  </si>
+  <si>
+    <t>Alfa64chan-29042020-004</t>
+  </si>
+  <si>
+    <t>Alfa64chan-29042020-005</t>
+  </si>
+  <si>
+    <t>Alfa64chan-29042020-006</t>
+  </si>
+  <si>
+    <t>Alfa64chan-29042020-007</t>
+  </si>
+  <si>
     <t>191119_Alfa_generate_parallel(3)</t>
   </si>
   <si>
@@ -3120,6 +3193,27 @@
     <t>200428_Alfa_selectivity_basic(2)</t>
   </si>
   <si>
+    <t>200429_Alfa_rfMapper_basic</t>
+  </si>
+  <si>
+    <t>200429_Alfa_generate_integrated</t>
+  </si>
+  <si>
+    <t>200429_Alfa_selectivity_basic</t>
+  </si>
+  <si>
+    <t>200429_Alfa_generate_integrated(1)</t>
+  </si>
+  <si>
+    <t>200429_Alfa_selectivity_basic(1)</t>
+  </si>
+  <si>
+    <t>200429_Alfa_generate_integrated(2)</t>
+  </si>
+  <si>
+    <t>200429_Alfa_selectivity_basic(2)</t>
+  </si>
+  <si>
     <t>N:\Stimuli\2019-06-Evolutions\alfa-191119a</t>
   </si>
   <si>
@@ -3655,6 +3749,24 @@
   </si>
   <si>
     <t>N:\Stimuli\2019-Manifold\alfa-200428c-selectivity</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-Manifold\alfa-200429a\2020-04-29-10-32-14</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-Manifold\alfa-200429a-selectivity</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-Manifold\alfa-200429b\2020-04-29-11-12-43</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-Manifold\alfa-200429b-selectivity</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-Manifold\alfa-200429c\2020-04-29-11-49-38</t>
+  </si>
+  <si>
+    <t>N:\Stimuli\2019-Manifold\alfa-200429c-selectivity</t>
   </si>
 </sst>
 </file>
@@ -4056,17 +4168,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H233"/>
+  <dimension ref="A1:H240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="G234" sqref="G234"/>
+    <sheetView tabSelected="1" topLeftCell="A226" workbookViewId="0">
+      <selection activeCell="G241" sqref="G241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="64.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" customWidth="1"/>
+    <col min="5" max="5" width="54.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4106,10 +4218,10 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="E2" t="s">
-        <v>476</v>
+        <v>490</v>
       </c>
       <c r="F2">
         <v>29</v>
@@ -4118,7 +4230,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>708</v>
+        <v>729</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4132,10 +4244,10 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="E3" t="s">
-        <v>477</v>
+        <v>491</v>
       </c>
       <c r="F3">
         <v>29</v>
@@ -4155,10 +4267,10 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="E4" t="s">
-        <v>478</v>
+        <v>492</v>
       </c>
       <c r="F4">
         <v>29</v>
@@ -4167,7 +4279,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>709</v>
+        <v>730</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4181,10 +4293,10 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="E5" t="s">
-        <v>479</v>
+        <v>493</v>
       </c>
       <c r="F5">
         <v>29</v>
@@ -4193,7 +4305,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>710</v>
+        <v>731</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4207,16 +4319,16 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="E6" t="s">
-        <v>480</v>
+        <v>494</v>
       </c>
       <c r="F6">
         <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>711</v>
+        <v>732</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4230,10 +4342,10 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="E7" t="s">
-        <v>481</v>
+        <v>495</v>
       </c>
       <c r="F7">
         <v>29</v>
@@ -4242,7 +4354,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>712</v>
+        <v>733</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4256,10 +4368,10 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="E8" t="s">
-        <v>482</v>
+        <v>496</v>
       </c>
       <c r="F8">
         <v>9</v>
@@ -4268,7 +4380,7 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>713</v>
+        <v>734</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4282,10 +4394,10 @@
         <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="E9" t="s">
-        <v>483</v>
+        <v>497</v>
       </c>
       <c r="F9">
         <v>9</v>
@@ -4294,7 +4406,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>714</v>
+        <v>735</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4308,10 +4420,10 @@
         <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="E10" t="s">
-        <v>484</v>
+        <v>498</v>
       </c>
       <c r="F10">
         <v>9</v>
@@ -4320,7 +4432,7 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>715</v>
+        <v>736</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4334,10 +4446,10 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="E11" t="s">
-        <v>485</v>
+        <v>499</v>
       </c>
       <c r="F11">
         <v>32</v>
@@ -4346,7 +4458,7 @@
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>716</v>
+        <v>737</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4360,10 +4472,10 @@
         <v>22</v>
       </c>
       <c r="D12" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E12" t="s">
-        <v>486</v>
+        <v>500</v>
       </c>
       <c r="F12">
         <v>32</v>
@@ -4372,7 +4484,7 @@
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>717</v>
+        <v>738</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4386,10 +4498,10 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="E13" t="s">
-        <v>487</v>
+        <v>501</v>
       </c>
       <c r="F13">
         <v>32</v>
@@ -4398,7 +4510,7 @@
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>718</v>
+        <v>739</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4406,10 +4518,10 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="E14" t="s">
-        <v>488</v>
+        <v>502</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4423,10 +4535,10 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="E15" t="s">
-        <v>489</v>
+        <v>503</v>
       </c>
       <c r="F15">
         <v>3</v>
@@ -4435,7 +4547,7 @@
         <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>719</v>
+        <v>740</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4449,10 +4561,10 @@
         <v>26</v>
       </c>
       <c r="D16" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="E16" t="s">
-        <v>490</v>
+        <v>504</v>
       </c>
       <c r="F16">
         <v>3</v>
@@ -4461,7 +4573,7 @@
         <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>720</v>
+        <v>741</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -4475,10 +4587,10 @@
         <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="E17" t="s">
-        <v>491</v>
+        <v>505</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -4487,7 +4599,7 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>721</v>
+        <v>742</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -4495,10 +4607,10 @@
         <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="E18" t="s">
-        <v>492</v>
+        <v>506</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -4512,10 +4624,10 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="E19" t="s">
-        <v>493</v>
+        <v>507</v>
       </c>
       <c r="F19">
         <v>7</v>
@@ -4524,7 +4636,7 @@
         <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>722</v>
+        <v>743</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -4538,10 +4650,10 @@
         <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="E20" t="s">
-        <v>494</v>
+        <v>508</v>
       </c>
       <c r="F20">
         <v>7</v>
@@ -4550,7 +4662,7 @@
         <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>723</v>
+        <v>744</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -4564,10 +4676,10 @@
         <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="E21" t="s">
-        <v>495</v>
+        <v>509</v>
       </c>
       <c r="F21">
         <v>7</v>
@@ -4576,7 +4688,7 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>724</v>
+        <v>745</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -4584,10 +4696,10 @@
         <v>32</v>
       </c>
       <c r="D22" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="E22" t="s">
-        <v>496</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -4595,16 +4707,16 @@
         <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="E23" t="s">
-        <v>497</v>
+        <v>511</v>
       </c>
       <c r="G23">
         <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>725</v>
+        <v>746</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -4612,16 +4724,16 @@
         <v>34</v>
       </c>
       <c r="D24" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="E24" t="s">
-        <v>498</v>
+        <v>512</v>
       </c>
       <c r="G24">
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>726</v>
+        <v>747</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -4629,10 +4741,10 @@
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="E25" t="s">
-        <v>499</v>
+        <v>513</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -4646,10 +4758,10 @@
         <v>36</v>
       </c>
       <c r="D26" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="E26" t="s">
-        <v>500</v>
+        <v>514</v>
       </c>
       <c r="F26">
         <v>51</v>
@@ -4658,7 +4770,7 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>727</v>
+        <v>748</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -4672,10 +4784,10 @@
         <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="E27" t="s">
-        <v>501</v>
+        <v>515</v>
       </c>
       <c r="F27">
         <v>51</v>
@@ -4684,7 +4796,7 @@
         <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>728</v>
+        <v>749</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -4698,10 +4810,10 @@
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="E28" t="s">
-        <v>502</v>
+        <v>516</v>
       </c>
       <c r="F28">
         <v>51</v>
@@ -4710,7 +4822,7 @@
         <v>3</v>
       </c>
       <c r="H28" t="s">
-        <v>729</v>
+        <v>750</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -4718,10 +4830,10 @@
         <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="E29" t="s">
-        <v>503</v>
+        <v>517</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -4735,10 +4847,10 @@
         <v>40</v>
       </c>
       <c r="D30" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="E30" t="s">
-        <v>504</v>
+        <v>518</v>
       </c>
       <c r="F30">
         <v>7</v>
@@ -4747,7 +4859,7 @@
         <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>730</v>
+        <v>751</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -4761,10 +4873,10 @@
         <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="E31" t="s">
-        <v>505</v>
+        <v>519</v>
       </c>
       <c r="F31">
         <v>7</v>
@@ -4773,7 +4885,7 @@
         <v>3</v>
       </c>
       <c r="H31" t="s">
-        <v>731</v>
+        <v>752</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -4787,10 +4899,10 @@
         <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="E32" t="s">
-        <v>506</v>
+        <v>520</v>
       </c>
       <c r="F32">
         <v>7</v>
@@ -4799,7 +4911,7 @@
         <v>3</v>
       </c>
       <c r="H32" t="s">
-        <v>732</v>
+        <v>753</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -4807,10 +4919,10 @@
         <v>43</v>
       </c>
       <c r="D33" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E33" t="s">
-        <v>507</v>
+        <v>521</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -4824,10 +4936,10 @@
         <v>44</v>
       </c>
       <c r="D34" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="E34" t="s">
-        <v>508</v>
+        <v>522</v>
       </c>
       <c r="F34">
         <v>7</v>
@@ -4836,7 +4948,7 @@
         <v>3</v>
       </c>
       <c r="H34" t="s">
-        <v>733</v>
+        <v>754</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -4850,10 +4962,10 @@
         <v>45</v>
       </c>
       <c r="D35" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="E35" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="F35">
         <v>7</v>
@@ -4862,7 +4974,7 @@
         <v>3</v>
       </c>
       <c r="H35" t="s">
-        <v>734</v>
+        <v>755</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -4876,10 +4988,10 @@
         <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="E36" t="s">
-        <v>510</v>
+        <v>524</v>
       </c>
       <c r="F36">
         <v>7</v>
@@ -4888,7 +5000,7 @@
         <v>3</v>
       </c>
       <c r="H36" t="s">
-        <v>735</v>
+        <v>756</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -4902,10 +5014,10 @@
         <v>47</v>
       </c>
       <c r="D37" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="E37" t="s">
-        <v>511</v>
+        <v>525</v>
       </c>
       <c r="F37">
         <v>36</v>
@@ -4914,7 +5026,7 @@
         <v>3</v>
       </c>
       <c r="H37" t="s">
-        <v>736</v>
+        <v>757</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -4928,10 +5040,10 @@
         <v>48</v>
       </c>
       <c r="D38" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="E38" t="s">
-        <v>512</v>
+        <v>526</v>
       </c>
       <c r="F38">
         <v>36</v>
@@ -4940,7 +5052,7 @@
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>737</v>
+        <v>758</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -4954,10 +5066,10 @@
         <v>49</v>
       </c>
       <c r="D39" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="E39" t="s">
-        <v>513</v>
+        <v>527</v>
       </c>
       <c r="F39">
         <v>35</v>
@@ -4966,7 +5078,7 @@
         <v>3</v>
       </c>
       <c r="H39" t="s">
-        <v>738</v>
+        <v>759</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -4980,10 +5092,10 @@
         <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="E40" t="s">
-        <v>514</v>
+        <v>528</v>
       </c>
       <c r="F40">
         <v>35</v>
@@ -4992,7 +5104,7 @@
         <v>3</v>
       </c>
       <c r="H40" t="s">
-        <v>739</v>
+        <v>760</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -5006,10 +5118,10 @@
         <v>51</v>
       </c>
       <c r="D41" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="E41" t="s">
-        <v>515</v>
+        <v>529</v>
       </c>
       <c r="F41">
         <v>35</v>
@@ -5018,7 +5130,7 @@
         <v>3</v>
       </c>
       <c r="H41" t="s">
-        <v>740</v>
+        <v>761</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -5032,10 +5144,10 @@
         <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="E42" t="s">
-        <v>516</v>
+        <v>530</v>
       </c>
       <c r="F42">
         <v>61</v>
@@ -5044,7 +5156,7 @@
         <v>3</v>
       </c>
       <c r="H42" t="s">
-        <v>741</v>
+        <v>762</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -5058,10 +5170,10 @@
         <v>53</v>
       </c>
       <c r="D43" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="E43" t="s">
-        <v>517</v>
+        <v>531</v>
       </c>
       <c r="F43">
         <v>61</v>
@@ -5070,7 +5182,7 @@
         <v>3</v>
       </c>
       <c r="H43" t="s">
-        <v>742</v>
+        <v>763</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -5084,10 +5196,10 @@
         <v>54</v>
       </c>
       <c r="D44" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="E44" t="s">
-        <v>518</v>
+        <v>532</v>
       </c>
       <c r="F44">
         <v>61</v>
@@ -5096,7 +5208,7 @@
         <v>3</v>
       </c>
       <c r="H44" t="s">
-        <v>743</v>
+        <v>764</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -5110,10 +5222,10 @@
         <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="E45" t="s">
-        <v>519</v>
+        <v>533</v>
       </c>
       <c r="F45">
         <v>33</v>
@@ -5122,7 +5234,7 @@
         <v>3</v>
       </c>
       <c r="H45" t="s">
-        <v>744</v>
+        <v>765</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -5136,10 +5248,10 @@
         <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="E46" t="s">
-        <v>520</v>
+        <v>534</v>
       </c>
       <c r="F46">
         <v>33</v>
@@ -5148,7 +5260,7 @@
         <v>3</v>
       </c>
       <c r="H46" t="s">
-        <v>745</v>
+        <v>766</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -5162,10 +5274,10 @@
         <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="E47" t="s">
-        <v>521</v>
+        <v>535</v>
       </c>
       <c r="F47">
         <v>33</v>
@@ -5174,7 +5286,7 @@
         <v>3</v>
       </c>
       <c r="H47" t="s">
-        <v>746</v>
+        <v>767</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -5188,10 +5300,10 @@
         <v>58</v>
       </c>
       <c r="D48" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="E48" t="s">
-        <v>522</v>
+        <v>536</v>
       </c>
       <c r="F48">
         <v>43</v>
@@ -5200,7 +5312,7 @@
         <v>3</v>
       </c>
       <c r="H48" t="s">
-        <v>747</v>
+        <v>768</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -5214,10 +5326,10 @@
         <v>59</v>
       </c>
       <c r="D49" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="E49" t="s">
-        <v>523</v>
+        <v>537</v>
       </c>
       <c r="F49">
         <v>43</v>
@@ -5226,7 +5338,7 @@
         <v>3</v>
       </c>
       <c r="H49" t="s">
-        <v>748</v>
+        <v>769</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -5240,10 +5352,10 @@
         <v>60</v>
       </c>
       <c r="D50" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="E50" t="s">
-        <v>524</v>
+        <v>538</v>
       </c>
       <c r="F50">
         <v>43</v>
@@ -5252,7 +5364,7 @@
         <v>3</v>
       </c>
       <c r="H50" t="s">
-        <v>749</v>
+        <v>770</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5266,10 +5378,10 @@
         <v>61</v>
       </c>
       <c r="D51" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="E51" t="s">
-        <v>525</v>
+        <v>539</v>
       </c>
       <c r="F51">
         <v>59</v>
@@ -5278,7 +5390,7 @@
         <v>3</v>
       </c>
       <c r="H51" t="s">
-        <v>750</v>
+        <v>771</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -5292,10 +5404,10 @@
         <v>62</v>
       </c>
       <c r="D52" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="E52" t="s">
-        <v>526</v>
+        <v>540</v>
       </c>
       <c r="F52">
         <v>59</v>
@@ -5304,7 +5416,7 @@
         <v>3</v>
       </c>
       <c r="H52" t="s">
-        <v>751</v>
+        <v>772</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -5318,10 +5430,10 @@
         <v>63</v>
       </c>
       <c r="D53" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="E53" t="s">
-        <v>527</v>
+        <v>541</v>
       </c>
       <c r="F53">
         <v>59</v>
@@ -5330,7 +5442,7 @@
         <v>3</v>
       </c>
       <c r="H53" t="s">
-        <v>752</v>
+        <v>773</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -5344,10 +5456,10 @@
         <v>64</v>
       </c>
       <c r="D54" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="E54" t="s">
-        <v>528</v>
+        <v>542</v>
       </c>
       <c r="F54">
         <v>20</v>
@@ -5356,7 +5468,7 @@
         <v>3</v>
       </c>
       <c r="H54" t="s">
-        <v>753</v>
+        <v>774</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -5370,10 +5482,10 @@
         <v>65</v>
       </c>
       <c r="D55" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="E55" t="s">
-        <v>529</v>
+        <v>543</v>
       </c>
       <c r="F55">
         <v>20</v>
@@ -5382,7 +5494,7 @@
         <v>3</v>
       </c>
       <c r="H55" t="s">
-        <v>754</v>
+        <v>775</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -5396,10 +5508,10 @@
         <v>66</v>
       </c>
       <c r="D56" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="E56" t="s">
-        <v>530</v>
+        <v>544</v>
       </c>
       <c r="F56">
         <v>20</v>
@@ -5408,7 +5520,7 @@
         <v>3</v>
       </c>
       <c r="H56" t="s">
-        <v>755</v>
+        <v>776</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -5422,10 +5534,10 @@
         <v>67</v>
       </c>
       <c r="D57" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="E57" t="s">
-        <v>531</v>
+        <v>545</v>
       </c>
       <c r="F57">
         <v>49</v>
@@ -5434,7 +5546,7 @@
         <v>3</v>
       </c>
       <c r="H57" t="s">
-        <v>756</v>
+        <v>777</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -5448,10 +5560,10 @@
         <v>68</v>
       </c>
       <c r="D58" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="E58" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="F58">
         <v>49</v>
@@ -5460,7 +5572,7 @@
         <v>3</v>
       </c>
       <c r="H58" t="s">
-        <v>757</v>
+        <v>778</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -5474,10 +5586,10 @@
         <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="E59" t="s">
-        <v>533</v>
+        <v>547</v>
       </c>
       <c r="F59">
         <v>49</v>
@@ -5486,7 +5598,7 @@
         <v>3</v>
       </c>
       <c r="H59" t="s">
-        <v>758</v>
+        <v>779</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -5500,10 +5612,10 @@
         <v>70</v>
       </c>
       <c r="D60" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="E60" t="s">
-        <v>534</v>
+        <v>548</v>
       </c>
       <c r="F60">
         <v>19</v>
@@ -5512,7 +5624,7 @@
         <v>3</v>
       </c>
       <c r="H60" t="s">
-        <v>759</v>
+        <v>780</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -5526,10 +5638,10 @@
         <v>71</v>
       </c>
       <c r="D61" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="E61" t="s">
-        <v>535</v>
+        <v>549</v>
       </c>
       <c r="F61">
         <v>19</v>
@@ -5538,7 +5650,7 @@
         <v>3</v>
       </c>
       <c r="H61" t="s">
-        <v>760</v>
+        <v>781</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -5552,10 +5664,10 @@
         <v>72</v>
       </c>
       <c r="D62" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="E62" t="s">
-        <v>536</v>
+        <v>550</v>
       </c>
       <c r="F62">
         <v>19</v>
@@ -5564,7 +5676,7 @@
         <v>3</v>
       </c>
       <c r="H62" t="s">
-        <v>761</v>
+        <v>782</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -5578,10 +5690,10 @@
         <v>73</v>
       </c>
       <c r="D63" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="E63" t="s">
-        <v>537</v>
+        <v>551</v>
       </c>
       <c r="F63">
         <v>12</v>
@@ -5590,7 +5702,7 @@
         <v>3</v>
       </c>
       <c r="H63" t="s">
-        <v>762</v>
+        <v>783</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -5604,10 +5716,10 @@
         <v>74</v>
       </c>
       <c r="D64" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="E64" t="s">
-        <v>538</v>
+        <v>552</v>
       </c>
       <c r="F64">
         <v>12</v>
@@ -5616,7 +5728,7 @@
         <v>3</v>
       </c>
       <c r="H64" t="s">
-        <v>763</v>
+        <v>784</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -5630,10 +5742,10 @@
         <v>75</v>
       </c>
       <c r="D65" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="E65" t="s">
-        <v>539</v>
+        <v>553</v>
       </c>
       <c r="F65">
         <v>12</v>
@@ -5642,7 +5754,7 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>764</v>
+        <v>785</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -5656,10 +5768,10 @@
         <v>76</v>
       </c>
       <c r="D66" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="E66" t="s">
-        <v>540</v>
+        <v>554</v>
       </c>
       <c r="F66">
         <v>41</v>
@@ -5668,7 +5780,7 @@
         <v>3</v>
       </c>
       <c r="H66" t="s">
-        <v>765</v>
+        <v>786</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -5682,10 +5794,10 @@
         <v>77</v>
       </c>
       <c r="D67" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="E67" t="s">
-        <v>541</v>
+        <v>555</v>
       </c>
       <c r="F67">
         <v>41</v>
@@ -5694,7 +5806,7 @@
         <v>3</v>
       </c>
       <c r="H67" t="s">
-        <v>766</v>
+        <v>787</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -5708,10 +5820,10 @@
         <v>78</v>
       </c>
       <c r="D68" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="E68" t="s">
-        <v>542</v>
+        <v>556</v>
       </c>
       <c r="F68">
         <v>41</v>
@@ -5720,7 +5832,7 @@
         <v>3</v>
       </c>
       <c r="H68" t="s">
-        <v>767</v>
+        <v>788</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -5734,10 +5846,10 @@
         <v>79</v>
       </c>
       <c r="D69" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="E69" t="s">
-        <v>543</v>
+        <v>557</v>
       </c>
       <c r="F69">
         <v>63</v>
@@ -5746,7 +5858,7 @@
         <v>3</v>
       </c>
       <c r="H69" t="s">
-        <v>768</v>
+        <v>789</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -5760,10 +5872,10 @@
         <v>80</v>
       </c>
       <c r="D70" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="E70" t="s">
-        <v>544</v>
+        <v>558</v>
       </c>
       <c r="F70">
         <v>63</v>
@@ -5772,7 +5884,7 @@
         <v>3</v>
       </c>
       <c r="H70" t="s">
-        <v>769</v>
+        <v>790</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -5786,10 +5898,10 @@
         <v>81</v>
       </c>
       <c r="D71" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E71" t="s">
-        <v>545</v>
+        <v>559</v>
       </c>
       <c r="F71">
         <v>63</v>
@@ -5798,7 +5910,7 @@
         <v>3</v>
       </c>
       <c r="H71" t="s">
-        <v>770</v>
+        <v>791</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -5812,10 +5924,10 @@
         <v>82</v>
       </c>
       <c r="D72" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="E72" t="s">
-        <v>546</v>
+        <v>560</v>
       </c>
       <c r="F72">
         <v>38</v>
@@ -5824,7 +5936,7 @@
         <v>3</v>
       </c>
       <c r="H72" t="s">
-        <v>771</v>
+        <v>792</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -5838,10 +5950,10 @@
         <v>83</v>
       </c>
       <c r="D73" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="E73" t="s">
-        <v>547</v>
+        <v>561</v>
       </c>
       <c r="F73">
         <v>38</v>
@@ -5850,7 +5962,7 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>772</v>
+        <v>793</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -5864,10 +5976,10 @@
         <v>84</v>
       </c>
       <c r="D74" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="E74" t="s">
-        <v>548</v>
+        <v>562</v>
       </c>
       <c r="F74">
         <v>38</v>
@@ -5876,7 +5988,7 @@
         <v>3</v>
       </c>
       <c r="H74" t="s">
-        <v>773</v>
+        <v>794</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -5890,10 +6002,10 @@
         <v>85</v>
       </c>
       <c r="D75" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="E75" t="s">
-        <v>549</v>
+        <v>563</v>
       </c>
       <c r="F75">
         <v>39</v>
@@ -5902,7 +6014,7 @@
         <v>3</v>
       </c>
       <c r="H75" t="s">
-        <v>774</v>
+        <v>795</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -5916,10 +6028,10 @@
         <v>86</v>
       </c>
       <c r="D76" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="E76" t="s">
-        <v>550</v>
+        <v>564</v>
       </c>
       <c r="F76">
         <v>39</v>
@@ -5928,7 +6040,7 @@
         <v>3</v>
       </c>
       <c r="H76" t="s">
-        <v>775</v>
+        <v>796</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -5942,10 +6054,10 @@
         <v>87</v>
       </c>
       <c r="D77" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="E77" t="s">
-        <v>551</v>
+        <v>565</v>
       </c>
       <c r="F77">
         <v>39</v>
@@ -5954,7 +6066,7 @@
         <v>3</v>
       </c>
       <c r="H77" t="s">
-        <v>776</v>
+        <v>797</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -5968,10 +6080,10 @@
         <v>88</v>
       </c>
       <c r="D78" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="E78" t="s">
-        <v>552</v>
+        <v>566</v>
       </c>
       <c r="F78">
         <v>44</v>
@@ -5980,7 +6092,7 @@
         <v>3</v>
       </c>
       <c r="H78" t="s">
-        <v>777</v>
+        <v>798</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -5994,10 +6106,10 @@
         <v>89</v>
       </c>
       <c r="D79" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="E79" t="s">
-        <v>553</v>
+        <v>567</v>
       </c>
       <c r="F79">
         <v>44</v>
@@ -6006,7 +6118,7 @@
         <v>3</v>
       </c>
       <c r="H79" t="s">
-        <v>778</v>
+        <v>799</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -6020,10 +6132,10 @@
         <v>90</v>
       </c>
       <c r="D80" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="E80" t="s">
-        <v>554</v>
+        <v>568</v>
       </c>
       <c r="F80">
         <v>44</v>
@@ -6032,7 +6144,7 @@
         <v>3</v>
       </c>
       <c r="H80" t="s">
-        <v>779</v>
+        <v>800</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -6043,13 +6155,13 @@
         <v>91</v>
       </c>
       <c r="D81" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="E81" t="s">
-        <v>555</v>
+        <v>569</v>
       </c>
       <c r="H81" t="s">
-        <v>780</v>
+        <v>801</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -6060,13 +6172,13 @@
         <v>92</v>
       </c>
       <c r="D82" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="E82" t="s">
-        <v>556</v>
+        <v>570</v>
       </c>
       <c r="H82" t="s">
-        <v>780</v>
+        <v>801</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -6080,10 +6192,10 @@
         <v>93</v>
       </c>
       <c r="D83" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="E83" t="s">
-        <v>557</v>
+        <v>571</v>
       </c>
       <c r="F83">
         <v>13</v>
@@ -6092,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="H83" t="s">
-        <v>781</v>
+        <v>802</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -6106,10 +6218,10 @@
         <v>94</v>
       </c>
       <c r="D84" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="E84" t="s">
-        <v>558</v>
+        <v>572</v>
       </c>
       <c r="F84">
         <v>28</v>
@@ -6118,7 +6230,7 @@
         <v>3</v>
       </c>
       <c r="H84" t="s">
-        <v>782</v>
+        <v>803</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -6132,10 +6244,10 @@
         <v>95</v>
       </c>
       <c r="D85" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="E85" t="s">
-        <v>559</v>
+        <v>573</v>
       </c>
       <c r="F85">
         <v>20</v>
@@ -6144,7 +6256,7 @@
         <v>5</v>
       </c>
       <c r="H85" t="s">
-        <v>783</v>
+        <v>804</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -6158,10 +6270,10 @@
         <v>96</v>
       </c>
       <c r="D86" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="E86" t="s">
-        <v>560</v>
+        <v>574</v>
       </c>
       <c r="F86">
         <v>48</v>
@@ -6170,7 +6282,7 @@
         <v>3</v>
       </c>
       <c r="H86" t="s">
-        <v>784</v>
+        <v>805</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -6181,13 +6293,13 @@
         <v>97</v>
       </c>
       <c r="D87" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="E87" t="s">
-        <v>561</v>
+        <v>575</v>
       </c>
       <c r="H87" t="s">
-        <v>785</v>
+        <v>806</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -6198,13 +6310,13 @@
         <v>98</v>
       </c>
       <c r="D88" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="E88" t="s">
-        <v>562</v>
+        <v>576</v>
       </c>
       <c r="H88" t="s">
-        <v>785</v>
+        <v>806</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -6218,10 +6330,10 @@
         <v>99</v>
       </c>
       <c r="D89" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="E89" t="s">
-        <v>563</v>
+        <v>577</v>
       </c>
       <c r="F89">
         <v>12</v>
@@ -6230,7 +6342,7 @@
         <v>3</v>
       </c>
       <c r="H89" t="s">
-        <v>786</v>
+        <v>807</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -6244,10 +6356,10 @@
         <v>100</v>
       </c>
       <c r="D90" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="E90" t="s">
-        <v>564</v>
+        <v>578</v>
       </c>
       <c r="F90">
         <v>12</v>
@@ -6256,7 +6368,7 @@
         <v>3</v>
       </c>
       <c r="H90" t="s">
-        <v>787</v>
+        <v>808</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -6270,10 +6382,10 @@
         <v>101</v>
       </c>
       <c r="D91" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="E91" t="s">
-        <v>565</v>
+        <v>579</v>
       </c>
       <c r="F91">
         <v>12</v>
@@ -6282,7 +6394,7 @@
         <v>3</v>
       </c>
       <c r="H91" t="s">
-        <v>788</v>
+        <v>809</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -6296,10 +6408,10 @@
         <v>102</v>
       </c>
       <c r="D92" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="E92" t="s">
-        <v>566</v>
+        <v>580</v>
       </c>
       <c r="F92">
         <v>12</v>
@@ -6308,7 +6420,7 @@
         <v>3</v>
       </c>
       <c r="H92" t="s">
-        <v>789</v>
+        <v>810</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -6322,10 +6434,10 @@
         <v>103</v>
       </c>
       <c r="D93" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="E93" t="s">
-        <v>567</v>
+        <v>581</v>
       </c>
       <c r="F93">
         <v>64</v>
@@ -6334,7 +6446,7 @@
         <v>4</v>
       </c>
       <c r="H93" t="s">
-        <v>790</v>
+        <v>811</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -6348,10 +6460,10 @@
         <v>104</v>
       </c>
       <c r="D94" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="E94" t="s">
-        <v>568</v>
+        <v>582</v>
       </c>
       <c r="F94">
         <v>64</v>
@@ -6360,7 +6472,7 @@
         <v>4</v>
       </c>
       <c r="H94" t="s">
-        <v>791</v>
+        <v>812</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -6371,13 +6483,13 @@
         <v>105</v>
       </c>
       <c r="D95" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="E95" t="s">
-        <v>569</v>
+        <v>583</v>
       </c>
       <c r="H95" t="s">
-        <v>792</v>
+        <v>813</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -6388,13 +6500,13 @@
         <v>106</v>
       </c>
       <c r="D96" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="E96" t="s">
-        <v>570</v>
+        <v>584</v>
       </c>
       <c r="H96" t="s">
-        <v>792</v>
+        <v>813</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -6408,10 +6520,10 @@
         <v>107</v>
       </c>
       <c r="D97" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="E97" t="s">
-        <v>571</v>
+        <v>585</v>
       </c>
       <c r="F97">
         <v>31</v>
@@ -6420,7 +6532,7 @@
         <v>4</v>
       </c>
       <c r="H97" t="s">
-        <v>793</v>
+        <v>814</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -6434,10 +6546,10 @@
         <v>108</v>
       </c>
       <c r="D98" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="E98" t="s">
-        <v>572</v>
+        <v>586</v>
       </c>
       <c r="F98">
         <v>21</v>
@@ -6446,7 +6558,7 @@
         <v>4</v>
       </c>
       <c r="H98" t="s">
-        <v>794</v>
+        <v>815</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -6460,10 +6572,10 @@
         <v>109</v>
       </c>
       <c r="D99" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="E99" t="s">
-        <v>573</v>
+        <v>587</v>
       </c>
       <c r="F99">
         <v>21</v>
@@ -6472,7 +6584,7 @@
         <v>4</v>
       </c>
       <c r="H99" t="s">
-        <v>795</v>
+        <v>816</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -6486,10 +6598,10 @@
         <v>110</v>
       </c>
       <c r="D100" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="E100" t="s">
-        <v>574</v>
+        <v>588</v>
       </c>
       <c r="F100">
         <v>21</v>
@@ -6498,7 +6610,7 @@
         <v>4</v>
       </c>
       <c r="H100" t="s">
-        <v>796</v>
+        <v>817</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -6512,10 +6624,10 @@
         <v>111</v>
       </c>
       <c r="D101" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="E101" t="s">
-        <v>575</v>
+        <v>589</v>
       </c>
       <c r="F101">
         <v>21</v>
@@ -6524,7 +6636,7 @@
         <v>4</v>
       </c>
       <c r="H101" t="s">
-        <v>797</v>
+        <v>818</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -6535,13 +6647,13 @@
         <v>112</v>
       </c>
       <c r="D102" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="E102" t="s">
-        <v>576</v>
+        <v>590</v>
       </c>
       <c r="H102" t="s">
-        <v>798</v>
+        <v>819</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -6552,13 +6664,13 @@
         <v>113</v>
       </c>
       <c r="D103" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="E103" t="s">
-        <v>577</v>
+        <v>591</v>
       </c>
       <c r="H103" t="s">
-        <v>798</v>
+        <v>819</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -6572,10 +6684,10 @@
         <v>114</v>
       </c>
       <c r="D104" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="E104" t="s">
-        <v>578</v>
+        <v>592</v>
       </c>
       <c r="F104">
         <v>30</v>
@@ -6584,7 +6696,7 @@
         <v>3</v>
       </c>
       <c r="H104" t="s">
-        <v>799</v>
+        <v>820</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -6598,10 +6710,10 @@
         <v>115</v>
       </c>
       <c r="D105" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="E105" t="s">
-        <v>579</v>
+        <v>593</v>
       </c>
       <c r="F105">
         <v>30</v>
@@ -6610,7 +6722,7 @@
         <v>3</v>
       </c>
       <c r="H105" t="s">
-        <v>800</v>
+        <v>821</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -6624,10 +6736,10 @@
         <v>116</v>
       </c>
       <c r="D106" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="E106" t="s">
-        <v>580</v>
+        <v>594</v>
       </c>
       <c r="F106">
         <v>58</v>
@@ -6636,7 +6748,7 @@
         <v>4</v>
       </c>
       <c r="H106" t="s">
-        <v>801</v>
+        <v>822</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
@@ -6650,10 +6762,10 @@
         <v>117</v>
       </c>
       <c r="D107" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="E107" t="s">
-        <v>581</v>
+        <v>595</v>
       </c>
       <c r="F107">
         <v>58</v>
@@ -6662,7 +6774,7 @@
         <v>4</v>
       </c>
       <c r="H107" t="s">
-        <v>802</v>
+        <v>823</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -6676,10 +6788,10 @@
         <v>118</v>
       </c>
       <c r="D108" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="E108" t="s">
-        <v>582</v>
+        <v>596</v>
       </c>
       <c r="F108">
         <v>34</v>
@@ -6688,7 +6800,7 @@
         <v>3</v>
       </c>
       <c r="H108" t="s">
-        <v>803</v>
+        <v>824</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -6699,13 +6811,13 @@
         <v>119</v>
       </c>
       <c r="D109" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="E109" t="s">
-        <v>583</v>
+        <v>597</v>
       </c>
       <c r="H109" t="s">
-        <v>804</v>
+        <v>825</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -6716,13 +6828,13 @@
         <v>120</v>
       </c>
       <c r="D110" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="E110" t="s">
-        <v>584</v>
+        <v>598</v>
       </c>
       <c r="H110" t="s">
-        <v>804</v>
+        <v>825</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -6736,13 +6848,13 @@
         <v>121</v>
       </c>
       <c r="D111" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="E111" t="s">
-        <v>585</v>
+        <v>599</v>
       </c>
       <c r="H111" t="s">
-        <v>805</v>
+        <v>826</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -6756,13 +6868,13 @@
         <v>122</v>
       </c>
       <c r="D112" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="E112" t="s">
-        <v>586</v>
+        <v>600</v>
       </c>
       <c r="H112" t="s">
-        <v>806</v>
+        <v>827</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -6776,13 +6888,13 @@
         <v>123</v>
       </c>
       <c r="D113" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="E113" t="s">
-        <v>587</v>
+        <v>601</v>
       </c>
       <c r="H113" t="s">
-        <v>807</v>
+        <v>828</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -6793,13 +6905,13 @@
         <v>124</v>
       </c>
       <c r="D114" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="E114" t="s">
-        <v>588</v>
+        <v>602</v>
       </c>
       <c r="H114" t="s">
-        <v>808</v>
+        <v>829</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
@@ -6810,13 +6922,13 @@
         <v>125</v>
       </c>
       <c r="D115" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="E115" t="s">
-        <v>589</v>
+        <v>603</v>
       </c>
       <c r="H115" t="s">
-        <v>808</v>
+        <v>829</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -6827,13 +6939,13 @@
         <v>126</v>
       </c>
       <c r="D116" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="E116" t="s">
-        <v>590</v>
+        <v>604</v>
       </c>
       <c r="H116" t="s">
-        <v>808</v>
+        <v>829</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -6847,13 +6959,13 @@
         <v>127</v>
       </c>
       <c r="D117" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="E117" t="s">
-        <v>591</v>
+        <v>605</v>
       </c>
       <c r="H117" t="s">
-        <v>809</v>
+        <v>830</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -6867,13 +6979,13 @@
         <v>128</v>
       </c>
       <c r="D118" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="E118" t="s">
-        <v>592</v>
+        <v>606</v>
       </c>
       <c r="H118" t="s">
-        <v>810</v>
+        <v>831</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -6887,13 +6999,13 @@
         <v>129</v>
       </c>
       <c r="D119" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="E119" t="s">
-        <v>593</v>
+        <v>607</v>
       </c>
       <c r="H119" t="s">
-        <v>811</v>
+        <v>832</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -6907,13 +7019,13 @@
         <v>130</v>
       </c>
       <c r="D120" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="E120" t="s">
-        <v>594</v>
+        <v>608</v>
       </c>
       <c r="H120" t="s">
-        <v>812</v>
+        <v>833</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -6924,10 +7036,10 @@
         <v>131</v>
       </c>
       <c r="D121" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="E121" t="s">
-        <v>595</v>
+        <v>609</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -6938,10 +7050,10 @@
         <v>132</v>
       </c>
       <c r="D122" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="E122" t="s">
-        <v>596</v>
+        <v>610</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -6952,10 +7064,10 @@
         <v>133</v>
       </c>
       <c r="D123" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="E123" t="s">
-        <v>597</v>
+        <v>611</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -6966,10 +7078,10 @@
         <v>134</v>
       </c>
       <c r="D124" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="E124" t="s">
-        <v>598</v>
+        <v>612</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -6983,13 +7095,13 @@
         <v>135</v>
       </c>
       <c r="D125" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="E125" t="s">
-        <v>599</v>
+        <v>613</v>
       </c>
       <c r="H125" t="s">
-        <v>813</v>
+        <v>834</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
@@ -7003,13 +7115,13 @@
         <v>136</v>
       </c>
       <c r="D126" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="E126" t="s">
-        <v>600</v>
+        <v>614</v>
       </c>
       <c r="H126" t="s">
-        <v>814</v>
+        <v>835</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -7023,13 +7135,13 @@
         <v>137</v>
       </c>
       <c r="D127" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="E127" t="s">
-        <v>601</v>
+        <v>615</v>
       </c>
       <c r="H127" t="s">
-        <v>815</v>
+        <v>836</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -7043,13 +7155,13 @@
         <v>138</v>
       </c>
       <c r="D128" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="E128" t="s">
-        <v>602</v>
+        <v>616</v>
       </c>
       <c r="H128" t="s">
-        <v>816</v>
+        <v>837</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -7063,13 +7175,13 @@
         <v>139</v>
       </c>
       <c r="D129" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="E129" t="s">
-        <v>603</v>
+        <v>617</v>
       </c>
       <c r="H129" t="s">
-        <v>817</v>
+        <v>838</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -7083,13 +7195,13 @@
         <v>140</v>
       </c>
       <c r="D130" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="E130" t="s">
-        <v>604</v>
+        <v>618</v>
       </c>
       <c r="H130" t="s">
-        <v>818</v>
+        <v>839</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -7103,13 +7215,13 @@
         <v>141</v>
       </c>
       <c r="D131" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="E131" t="s">
-        <v>605</v>
+        <v>619</v>
       </c>
       <c r="H131" t="s">
-        <v>819</v>
+        <v>840</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -7123,13 +7235,13 @@
         <v>142</v>
       </c>
       <c r="D132" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="E132" t="s">
-        <v>606</v>
+        <v>620</v>
       </c>
       <c r="H132" t="s">
-        <v>820</v>
+        <v>841</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -7143,13 +7255,13 @@
         <v>143</v>
       </c>
       <c r="D133" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="E133" t="s">
-        <v>607</v>
+        <v>621</v>
       </c>
       <c r="H133" t="s">
-        <v>821</v>
+        <v>842</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
@@ -7157,13 +7269,13 @@
         <v>144</v>
       </c>
       <c r="D134" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="E134" t="s">
-        <v>608</v>
+        <v>622</v>
       </c>
       <c r="H134" t="s">
-        <v>822</v>
+        <v>843</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -7174,13 +7286,13 @@
         <v>145</v>
       </c>
       <c r="D135" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="E135" t="s">
-        <v>609</v>
+        <v>623</v>
       </c>
       <c r="H135" t="s">
-        <v>823</v>
+        <v>844</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -7188,10 +7300,10 @@
         <v>146</v>
       </c>
       <c r="D136" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="E136" t="s">
-        <v>610</v>
+        <v>624</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -7205,13 +7317,13 @@
         <v>147</v>
       </c>
       <c r="D137" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="E137" t="s">
-        <v>611</v>
+        <v>625</v>
       </c>
       <c r="H137" t="s">
-        <v>824</v>
+        <v>845</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -7222,10 +7334,10 @@
         <v>148</v>
       </c>
       <c r="D138" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="E138" t="s">
-        <v>612</v>
+        <v>626</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -7236,10 +7348,10 @@
         <v>149</v>
       </c>
       <c r="D139" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="E139" t="s">
-        <v>613</v>
+        <v>627</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -7253,13 +7365,13 @@
         <v>150</v>
       </c>
       <c r="D140" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="E140" t="s">
-        <v>614</v>
+        <v>628</v>
       </c>
       <c r="H140" t="s">
-        <v>825</v>
+        <v>846</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -7270,10 +7382,10 @@
         <v>151</v>
       </c>
       <c r="D141" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="E141" t="s">
-        <v>615</v>
+        <v>629</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -7284,10 +7396,10 @@
         <v>152</v>
       </c>
       <c r="D142" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="E142" t="s">
-        <v>616</v>
+        <v>630</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -7301,13 +7413,13 @@
         <v>153</v>
       </c>
       <c r="D143" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="E143" t="s">
-        <v>617</v>
+        <v>631</v>
       </c>
       <c r="H143" t="s">
-        <v>826</v>
+        <v>847</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -7318,10 +7430,10 @@
         <v>154</v>
       </c>
       <c r="D144" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="E144" t="s">
-        <v>618</v>
+        <v>632</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -7332,10 +7444,10 @@
         <v>155</v>
       </c>
       <c r="D145" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="E145" t="s">
-        <v>619</v>
+        <v>633</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
@@ -7349,13 +7461,13 @@
         <v>156</v>
       </c>
       <c r="D146" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="E146" t="s">
-        <v>620</v>
+        <v>634</v>
       </c>
       <c r="H146" t="s">
-        <v>827</v>
+        <v>848</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -7366,10 +7478,10 @@
         <v>157</v>
       </c>
       <c r="D147" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="E147" t="s">
-        <v>621</v>
+        <v>635</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -7380,10 +7492,10 @@
         <v>158</v>
       </c>
       <c r="D148" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="E148" t="s">
-        <v>622</v>
+        <v>636</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -7397,13 +7509,13 @@
         <v>159</v>
       </c>
       <c r="D149" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="E149" t="s">
-        <v>623</v>
+        <v>637</v>
       </c>
       <c r="H149" t="s">
-        <v>828</v>
+        <v>849</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -7417,13 +7529,13 @@
         <v>160</v>
       </c>
       <c r="D150" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="E150" t="s">
-        <v>624</v>
+        <v>638</v>
       </c>
       <c r="H150" t="s">
-        <v>829</v>
+        <v>850</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -7437,13 +7549,13 @@
         <v>161</v>
       </c>
       <c r="D151" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="E151" t="s">
-        <v>625</v>
+        <v>639</v>
       </c>
       <c r="H151" t="s">
-        <v>830</v>
+        <v>851</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -7454,10 +7566,10 @@
         <v>162</v>
       </c>
       <c r="D152" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="E152" t="s">
-        <v>626</v>
+        <v>640</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -7468,10 +7580,10 @@
         <v>163</v>
       </c>
       <c r="D153" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="E153" t="s">
-        <v>627</v>
+        <v>641</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -7485,13 +7597,13 @@
         <v>164</v>
       </c>
       <c r="D154" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="E154" t="s">
-        <v>628</v>
+        <v>642</v>
       </c>
       <c r="H154" t="s">
-        <v>831</v>
+        <v>852</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -7502,10 +7614,10 @@
         <v>165</v>
       </c>
       <c r="D155" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="E155" t="s">
-        <v>629</v>
+        <v>643</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -7516,10 +7628,10 @@
         <v>166</v>
       </c>
       <c r="D156" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="E156" t="s">
-        <v>630</v>
+        <v>644</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -7533,13 +7645,13 @@
         <v>167</v>
       </c>
       <c r="D157" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="E157" t="s">
-        <v>631</v>
+        <v>645</v>
       </c>
       <c r="H157" t="s">
-        <v>832</v>
+        <v>853</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -7553,13 +7665,13 @@
         <v>168</v>
       </c>
       <c r="D158" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="E158" t="s">
-        <v>632</v>
+        <v>646</v>
       </c>
       <c r="H158" t="s">
-        <v>833</v>
+        <v>854</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -7570,10 +7682,10 @@
         <v>169</v>
       </c>
       <c r="D159" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="E159" t="s">
-        <v>633</v>
+        <v>647</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -7584,10 +7696,10 @@
         <v>170</v>
       </c>
       <c r="D160" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="E160" t="s">
-        <v>634</v>
+        <v>648</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -7601,13 +7713,13 @@
         <v>171</v>
       </c>
       <c r="D161" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="E161" t="s">
-        <v>635</v>
+        <v>649</v>
       </c>
       <c r="H161" t="s">
-        <v>834</v>
+        <v>855</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -7621,13 +7733,13 @@
         <v>172</v>
       </c>
       <c r="D162" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="E162" t="s">
-        <v>636</v>
+        <v>650</v>
       </c>
       <c r="H162" t="s">
-        <v>835</v>
+        <v>856</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -7641,13 +7753,13 @@
         <v>173</v>
       </c>
       <c r="D163" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="E163" t="s">
-        <v>637</v>
+        <v>651</v>
       </c>
       <c r="H163" t="s">
-        <v>836</v>
+        <v>857</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -7658,10 +7770,10 @@
         <v>174</v>
       </c>
       <c r="D164" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="E164" t="s">
-        <v>638</v>
+        <v>652</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -7672,10 +7784,10 @@
         <v>175</v>
       </c>
       <c r="D165" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="E165" t="s">
-        <v>639</v>
+        <v>653</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -7689,13 +7801,13 @@
         <v>176</v>
       </c>
       <c r="D166" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="E166" t="s">
-        <v>640</v>
+        <v>654</v>
       </c>
       <c r="H166" t="s">
-        <v>837</v>
+        <v>858</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -7709,13 +7821,13 @@
         <v>177</v>
       </c>
       <c r="D167" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="E167" t="s">
-        <v>641</v>
+        <v>655</v>
       </c>
       <c r="H167" t="s">
-        <v>838</v>
+        <v>859</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
@@ -7726,10 +7838,10 @@
         <v>178</v>
       </c>
       <c r="D168" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="E168" t="s">
-        <v>642</v>
+        <v>656</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
@@ -7740,10 +7852,10 @@
         <v>179</v>
       </c>
       <c r="D169" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="E169" t="s">
-        <v>643</v>
+        <v>657</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -7757,13 +7869,13 @@
         <v>180</v>
       </c>
       <c r="D170" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="E170" t="s">
-        <v>644</v>
+        <v>658</v>
       </c>
       <c r="H170" t="s">
-        <v>839</v>
+        <v>860</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -7777,13 +7889,13 @@
         <v>181</v>
       </c>
       <c r="D171" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="E171" t="s">
-        <v>645</v>
+        <v>659</v>
       </c>
       <c r="H171" t="s">
-        <v>840</v>
+        <v>861</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
@@ -7797,13 +7909,13 @@
         <v>182</v>
       </c>
       <c r="D172" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="E172" t="s">
-        <v>646</v>
+        <v>660</v>
       </c>
       <c r="H172" t="s">
-        <v>841</v>
+        <v>862</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -7817,13 +7929,13 @@
         <v>183</v>
       </c>
       <c r="D173" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="E173" t="s">
-        <v>647</v>
+        <v>661</v>
       </c>
       <c r="H173" t="s">
-        <v>842</v>
+        <v>863</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -7837,13 +7949,13 @@
         <v>184</v>
       </c>
       <c r="D174" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="E174" t="s">
-        <v>648</v>
+        <v>662</v>
       </c>
       <c r="H174" t="s">
-        <v>843</v>
+        <v>864</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
@@ -7854,13 +7966,13 @@
         <v>185</v>
       </c>
       <c r="D175" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="E175" t="s">
-        <v>649</v>
+        <v>663</v>
       </c>
       <c r="H175" t="s">
-        <v>844</v>
+        <v>865</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -7871,10 +7983,10 @@
         <v>186</v>
       </c>
       <c r="D176" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="E176" t="s">
-        <v>650</v>
+        <v>664</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -7885,10 +7997,10 @@
         <v>187</v>
       </c>
       <c r="D177" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="E177" t="s">
-        <v>651</v>
+        <v>665</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -7899,10 +8011,10 @@
         <v>188</v>
       </c>
       <c r="D178" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="E178" t="s">
-        <v>652</v>
+        <v>666</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
@@ -7916,13 +8028,13 @@
         <v>189</v>
       </c>
       <c r="D179" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="E179" t="s">
-        <v>653</v>
+        <v>667</v>
       </c>
       <c r="H179" t="s">
-        <v>845</v>
+        <v>866</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -7936,13 +8048,13 @@
         <v>190</v>
       </c>
       <c r="D180" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="E180" t="s">
-        <v>654</v>
+        <v>668</v>
       </c>
       <c r="H180" t="s">
-        <v>846</v>
+        <v>867</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -7953,13 +8065,13 @@
         <v>191</v>
       </c>
       <c r="D181" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="E181" t="s">
-        <v>655</v>
+        <v>669</v>
       </c>
       <c r="H181" t="s">
-        <v>847</v>
+        <v>868</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
@@ -7970,10 +8082,10 @@
         <v>192</v>
       </c>
       <c r="D182" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="E182" t="s">
-        <v>656</v>
+        <v>670</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
@@ -7984,10 +8096,10 @@
         <v>193</v>
       </c>
       <c r="D183" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="E183" t="s">
-        <v>657</v>
+        <v>671</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
@@ -8001,10 +8113,10 @@
         <v>194</v>
       </c>
       <c r="D184" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="E184" t="s">
-        <v>658</v>
+        <v>672</v>
       </c>
       <c r="F184">
         <v>4</v>
@@ -8013,7 +8125,7 @@
         <v>4</v>
       </c>
       <c r="H184" t="s">
-        <v>848</v>
+        <v>869</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
@@ -8027,10 +8139,10 @@
         <v>195</v>
       </c>
       <c r="D185" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="E185" t="s">
-        <v>659</v>
+        <v>673</v>
       </c>
       <c r="F185">
         <v>4</v>
@@ -8039,7 +8151,7 @@
         <v>4</v>
       </c>
       <c r="H185" t="s">
-        <v>849</v>
+        <v>870</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
@@ -8053,10 +8165,10 @@
         <v>196</v>
       </c>
       <c r="D186" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="E186" t="s">
-        <v>660</v>
+        <v>674</v>
       </c>
       <c r="F186">
         <v>46</v>
@@ -8065,7 +8177,7 @@
         <v>2</v>
       </c>
       <c r="H186" t="s">
-        <v>850</v>
+        <v>871</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
@@ -8079,10 +8191,10 @@
         <v>197</v>
       </c>
       <c r="D187" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="E187" t="s">
-        <v>661</v>
+        <v>675</v>
       </c>
       <c r="F187">
         <v>46</v>
@@ -8091,7 +8203,7 @@
         <v>2</v>
       </c>
       <c r="H187" t="s">
-        <v>851</v>
+        <v>872</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
@@ -8102,10 +8214,10 @@
         <v>198</v>
       </c>
       <c r="D188" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="E188" t="s">
-        <v>662</v>
+        <v>676</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
@@ -8116,10 +8228,10 @@
         <v>199</v>
       </c>
       <c r="D189" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="E189" t="s">
-        <v>663</v>
+        <v>677</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
@@ -8133,10 +8245,10 @@
         <v>200</v>
       </c>
       <c r="D190" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="E190" t="s">
-        <v>664</v>
+        <v>678</v>
       </c>
       <c r="F190">
         <v>27</v>
@@ -8145,7 +8257,7 @@
         <v>6</v>
       </c>
       <c r="H190" t="s">
-        <v>852</v>
+        <v>873</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
@@ -8159,10 +8271,10 @@
         <v>201</v>
       </c>
       <c r="D191" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="E191" t="s">
-        <v>665</v>
+        <v>679</v>
       </c>
       <c r="F191">
         <v>27</v>
@@ -8171,7 +8283,7 @@
         <v>6</v>
       </c>
       <c r="H191" t="s">
-        <v>853</v>
+        <v>874</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
@@ -8185,10 +8297,10 @@
         <v>202</v>
       </c>
       <c r="D192" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="E192" t="s">
-        <v>666</v>
+        <v>680</v>
       </c>
       <c r="F192">
         <v>58</v>
@@ -8197,7 +8309,7 @@
         <v>2</v>
       </c>
       <c r="H192" t="s">
-        <v>854</v>
+        <v>875</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -8211,10 +8323,10 @@
         <v>203</v>
       </c>
       <c r="D193" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="E193" t="s">
-        <v>667</v>
+        <v>681</v>
       </c>
       <c r="F193">
         <v>58</v>
@@ -8223,7 +8335,7 @@
         <v>2</v>
       </c>
       <c r="H193" t="s">
-        <v>855</v>
+        <v>876</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -8234,10 +8346,10 @@
         <v>204</v>
       </c>
       <c r="D194" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="E194" t="s">
-        <v>668</v>
+        <v>682</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
@@ -8248,10 +8360,10 @@
         <v>205</v>
       </c>
       <c r="D195" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="E195" t="s">
-        <v>669</v>
+        <v>683</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
@@ -8265,10 +8377,10 @@
         <v>206</v>
       </c>
       <c r="D196" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="E196" t="s">
-        <v>670</v>
+        <v>684</v>
       </c>
       <c r="F196">
         <v>1</v>
@@ -8277,7 +8389,7 @@
         <v>5</v>
       </c>
       <c r="H196" t="s">
-        <v>856</v>
+        <v>877</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
@@ -8291,10 +8403,10 @@
         <v>207</v>
       </c>
       <c r="D197" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="E197" t="s">
-        <v>671</v>
+        <v>685</v>
       </c>
       <c r="F197">
         <v>1</v>
@@ -8303,7 +8415,7 @@
         <v>5</v>
       </c>
       <c r="H197" t="s">
-        <v>857</v>
+        <v>878</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
@@ -8317,10 +8429,10 @@
         <v>208</v>
       </c>
       <c r="D198" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="E198" t="s">
-        <v>672</v>
+        <v>686</v>
       </c>
       <c r="F198">
         <v>53</v>
@@ -8329,7 +8441,7 @@
         <v>3</v>
       </c>
       <c r="H198" t="s">
-        <v>858</v>
+        <v>879</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
@@ -8343,10 +8455,10 @@
         <v>209</v>
       </c>
       <c r="D199" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="E199" t="s">
-        <v>673</v>
+        <v>687</v>
       </c>
       <c r="F199">
         <v>53</v>
@@ -8355,7 +8467,7 @@
         <v>3</v>
       </c>
       <c r="H199" t="s">
-        <v>859</v>
+        <v>880</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
@@ -8369,10 +8481,10 @@
         <v>210</v>
       </c>
       <c r="D200" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="E200" t="s">
-        <v>674</v>
+        <v>688</v>
       </c>
       <c r="F200">
         <v>37</v>
@@ -8381,7 +8493,7 @@
         <v>2</v>
       </c>
       <c r="H200" t="s">
-        <v>860</v>
+        <v>881</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
@@ -8395,10 +8507,10 @@
         <v>211</v>
       </c>
       <c r="D201" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="E201" t="s">
-        <v>675</v>
+        <v>689</v>
       </c>
       <c r="F201">
         <v>37</v>
@@ -8407,7 +8519,7 @@
         <v>2</v>
       </c>
       <c r="H201" t="s">
-        <v>861</v>
+        <v>882</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.25">
@@ -8418,10 +8530,10 @@
         <v>212</v>
       </c>
       <c r="D202" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="E202" t="s">
-        <v>676</v>
+        <v>690</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.25">
@@ -8432,10 +8544,10 @@
         <v>213</v>
       </c>
       <c r="D203" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="E203" t="s">
-        <v>677</v>
+        <v>691</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.25">
@@ -8449,10 +8561,10 @@
         <v>214</v>
       </c>
       <c r="D204" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="E204" t="s">
-        <v>678</v>
+        <v>692</v>
       </c>
       <c r="F204">
         <v>8</v>
@@ -8461,7 +8573,7 @@
         <v>3</v>
       </c>
       <c r="H204" t="s">
-        <v>862</v>
+        <v>883</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.25">
@@ -8475,10 +8587,10 @@
         <v>215</v>
       </c>
       <c r="D205" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="E205" t="s">
-        <v>679</v>
+        <v>693</v>
       </c>
       <c r="F205">
         <v>8</v>
@@ -8487,7 +8599,7 @@
         <v>3</v>
       </c>
       <c r="H205" t="s">
-        <v>863</v>
+        <v>884</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.25">
@@ -8501,10 +8613,10 @@
         <v>216</v>
       </c>
       <c r="D206" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="E206" t="s">
-        <v>680</v>
+        <v>694</v>
       </c>
       <c r="F206">
         <v>50</v>
@@ -8513,7 +8625,7 @@
         <v>3</v>
       </c>
       <c r="H206" t="s">
-        <v>864</v>
+        <v>885</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.25">
@@ -8527,10 +8639,10 @@
         <v>217</v>
       </c>
       <c r="D207" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="E207" t="s">
-        <v>681</v>
+        <v>695</v>
       </c>
       <c r="F207">
         <v>50</v>
@@ -8539,7 +8651,7 @@
         <v>3</v>
       </c>
       <c r="H207" t="s">
-        <v>865</v>
+        <v>886</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.25">
@@ -8550,13 +8662,13 @@
         <v>218</v>
       </c>
       <c r="D208" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="E208" t="s">
-        <v>682</v>
+        <v>696</v>
       </c>
       <c r="H208" t="s">
-        <v>866</v>
+        <v>887</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.25">
@@ -8567,10 +8679,10 @@
         <v>219</v>
       </c>
       <c r="D209" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="E209" t="s">
-        <v>683</v>
+        <v>697</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.25">
@@ -8584,10 +8696,10 @@
         <v>220</v>
       </c>
       <c r="D210" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="E210" t="s">
-        <v>684</v>
+        <v>698</v>
       </c>
       <c r="F210">
         <v>62</v>
@@ -8596,7 +8708,7 @@
         <v>3</v>
       </c>
       <c r="H210" t="s">
-        <v>867</v>
+        <v>888</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">
@@ -8610,10 +8722,10 @@
         <v>221</v>
       </c>
       <c r="D211" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="E211" t="s">
-        <v>685</v>
+        <v>699</v>
       </c>
       <c r="F211">
         <v>62</v>
@@ -8622,7 +8734,7 @@
         <v>3</v>
       </c>
       <c r="H211" t="s">
-        <v>868</v>
+        <v>889</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.25">
@@ -8636,10 +8748,10 @@
         <v>222</v>
       </c>
       <c r="D212" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="E212" t="s">
-        <v>686</v>
+        <v>700</v>
       </c>
       <c r="F212">
         <v>48</v>
@@ -8648,7 +8760,7 @@
         <v>2</v>
       </c>
       <c r="H212" t="s">
-        <v>869</v>
+        <v>890</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.25">
@@ -8662,10 +8774,10 @@
         <v>223</v>
       </c>
       <c r="D213" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="E213" t="s">
-        <v>687</v>
+        <v>701</v>
       </c>
       <c r="F213">
         <v>48</v>
@@ -8674,7 +8786,7 @@
         <v>2</v>
       </c>
       <c r="H213" t="s">
-        <v>870</v>
+        <v>891</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.25">
@@ -8688,10 +8800,10 @@
         <v>224</v>
       </c>
       <c r="D214" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="E214" t="s">
-        <v>688</v>
+        <v>702</v>
       </c>
       <c r="F214">
         <v>45</v>
@@ -8700,7 +8812,7 @@
         <v>2</v>
       </c>
       <c r="H214" t="s">
-        <v>871</v>
+        <v>892</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.25">
@@ -8714,10 +8826,10 @@
         <v>225</v>
       </c>
       <c r="D215" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="E215" t="s">
-        <v>689</v>
+        <v>703</v>
       </c>
       <c r="F215">
         <v>45</v>
@@ -8726,7 +8838,7 @@
         <v>2</v>
       </c>
       <c r="H215" t="s">
-        <v>872</v>
+        <v>893</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.25">
@@ -8737,10 +8849,10 @@
         <v>226</v>
       </c>
       <c r="D216" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="E216" t="s">
-        <v>690</v>
+        <v>704</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.25">
@@ -8754,10 +8866,10 @@
         <v>227</v>
       </c>
       <c r="D217" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="E217" t="s">
-        <v>691</v>
+        <v>705</v>
       </c>
       <c r="F217">
         <v>2</v>
@@ -8766,7 +8878,7 @@
         <v>3</v>
       </c>
       <c r="H217" t="s">
-        <v>873</v>
+        <v>894</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.25">
@@ -8780,10 +8892,10 @@
         <v>228</v>
       </c>
       <c r="D218" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="E218" t="s">
-        <v>692</v>
+        <v>706</v>
       </c>
       <c r="F218">
         <v>2</v>
@@ -8792,7 +8904,7 @@
         <v>3</v>
       </c>
       <c r="H218" t="s">
-        <v>874</v>
+        <v>895</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.25">
@@ -8806,10 +8918,10 @@
         <v>229</v>
       </c>
       <c r="D219" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="E219" t="s">
-        <v>693</v>
+        <v>707</v>
       </c>
       <c r="F219">
         <v>19</v>
@@ -8818,7 +8930,7 @@
         <v>6</v>
       </c>
       <c r="H219" t="s">
-        <v>875</v>
+        <v>896</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.25">
@@ -8826,10 +8938,10 @@
         <v>230</v>
       </c>
       <c r="D220" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="E220" t="s">
-        <v>694</v>
+        <v>708</v>
       </c>
       <c r="F220">
         <v>19</v>
@@ -8849,10 +8961,10 @@
         <v>231</v>
       </c>
       <c r="D221" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="E221" t="s">
-        <v>695</v>
+        <v>709</v>
       </c>
       <c r="F221">
         <v>19</v>
@@ -8861,7 +8973,7 @@
         <v>6</v>
       </c>
       <c r="H221" t="s">
-        <v>876</v>
+        <v>897</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.25">
@@ -8872,10 +8984,10 @@
         <v>232</v>
       </c>
       <c r="D222" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="E222" t="s">
-        <v>696</v>
+        <v>710</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.25">
@@ -8889,10 +9001,10 @@
         <v>233</v>
       </c>
       <c r="D223" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="E223" t="s">
-        <v>697</v>
+        <v>711</v>
       </c>
       <c r="F223">
         <v>5</v>
@@ -8901,7 +9013,7 @@
         <v>3</v>
       </c>
       <c r="H223" t="s">
-        <v>877</v>
+        <v>898</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.25">
@@ -8915,10 +9027,10 @@
         <v>234</v>
       </c>
       <c r="D224" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="E224" t="s">
-        <v>698</v>
+        <v>712</v>
       </c>
       <c r="F224">
         <v>5</v>
@@ -8927,7 +9039,7 @@
         <v>3</v>
       </c>
       <c r="H224" t="s">
-        <v>878</v>
+        <v>899</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.25">
@@ -8941,10 +9053,10 @@
         <v>235</v>
       </c>
       <c r="D225" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="E225" t="s">
-        <v>699</v>
+        <v>713</v>
       </c>
       <c r="F225">
         <v>15</v>
@@ -8953,7 +9065,7 @@
         <v>3</v>
       </c>
       <c r="H225" t="s">
-        <v>879</v>
+        <v>900</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.25">
@@ -8967,10 +9079,10 @@
         <v>236</v>
       </c>
       <c r="D226" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="E226" t="s">
-        <v>700</v>
+        <v>714</v>
       </c>
       <c r="F226">
         <v>15</v>
@@ -8979,7 +9091,7 @@
         <v>3</v>
       </c>
       <c r="H226" t="s">
-        <v>880</v>
+        <v>901</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.25">
@@ -8990,10 +9102,10 @@
         <v>237</v>
       </c>
       <c r="D227" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="E227" t="s">
-        <v>701</v>
+        <v>715</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.25">
@@ -9007,10 +9119,10 @@
         <v>238</v>
       </c>
       <c r="D228" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="E228" t="s">
-        <v>702</v>
+        <v>716</v>
       </c>
       <c r="F228">
         <v>30</v>
@@ -9019,7 +9131,7 @@
         <v>4</v>
       </c>
       <c r="H228" t="s">
-        <v>881</v>
+        <v>902</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.25">
@@ -9033,10 +9145,10 @@
         <v>239</v>
       </c>
       <c r="D229" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="E229" t="s">
-        <v>703</v>
+        <v>717</v>
       </c>
       <c r="F229">
         <v>30</v>
@@ -9045,7 +9157,7 @@
         <v>4</v>
       </c>
       <c r="H229" t="s">
-        <v>882</v>
+        <v>903</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.25">
@@ -9059,10 +9171,10 @@
         <v>240</v>
       </c>
       <c r="D230" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="E230" t="s">
-        <v>704</v>
+        <v>718</v>
       </c>
       <c r="F230">
         <v>16</v>
@@ -9071,7 +9183,7 @@
         <v>3</v>
       </c>
       <c r="H230" t="s">
-        <v>883</v>
+        <v>904</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.25">
@@ -9085,10 +9197,10 @@
         <v>241</v>
       </c>
       <c r="D231" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="E231" t="s">
-        <v>705</v>
+        <v>719</v>
       </c>
       <c r="F231">
         <v>16</v>
@@ -9097,7 +9209,7 @@
         <v>3</v>
       </c>
       <c r="H231" t="s">
-        <v>884</v>
+        <v>905</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">
@@ -9111,10 +9223,10 @@
         <v>242</v>
       </c>
       <c r="D232" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="E232" t="s">
-        <v>706</v>
+        <v>720</v>
       </c>
       <c r="F232">
         <v>52</v>
@@ -9123,7 +9235,7 @@
         <v>4</v>
       </c>
       <c r="H232" t="s">
-        <v>885</v>
+        <v>906</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.25">
@@ -9137,10 +9249,10 @@
         <v>243</v>
       </c>
       <c r="D233" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="E233" t="s">
-        <v>707</v>
+        <v>721</v>
       </c>
       <c r="F233">
         <v>52</v>
@@ -9149,7 +9261,177 @@
         <v>4</v>
       </c>
       <c r="H233" t="s">
-        <v>886</v>
+        <v>907</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>8</v>
+      </c>
+      <c r="C234" t="s">
+        <v>244</v>
+      </c>
+      <c r="D234" t="s">
+        <v>483</v>
+      </c>
+      <c r="E234" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>8</v>
+      </c>
+      <c r="B235">
+        <v>44</v>
+      </c>
+      <c r="C235" t="s">
+        <v>245</v>
+      </c>
+      <c r="D235" t="s">
+        <v>484</v>
+      </c>
+      <c r="E235" t="s">
+        <v>723</v>
+      </c>
+      <c r="F235">
+        <v>54</v>
+      </c>
+      <c r="G235">
+        <v>3</v>
+      </c>
+      <c r="H235" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>8</v>
+      </c>
+      <c r="B236">
+        <v>44</v>
+      </c>
+      <c r="C236" t="s">
+        <v>246</v>
+      </c>
+      <c r="D236" t="s">
+        <v>485</v>
+      </c>
+      <c r="E236" t="s">
+        <v>724</v>
+      </c>
+      <c r="F236">
+        <v>54</v>
+      </c>
+      <c r="G236">
+        <v>3</v>
+      </c>
+      <c r="H236" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>8</v>
+      </c>
+      <c r="B237">
+        <v>45</v>
+      </c>
+      <c r="C237" t="s">
+        <v>247</v>
+      </c>
+      <c r="D237" t="s">
+        <v>486</v>
+      </c>
+      <c r="E237" t="s">
+        <v>725</v>
+      </c>
+      <c r="F237">
+        <v>57</v>
+      </c>
+      <c r="G237">
+        <v>2</v>
+      </c>
+      <c r="H237" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>8</v>
+      </c>
+      <c r="B238">
+        <v>45</v>
+      </c>
+      <c r="C238" t="s">
+        <v>248</v>
+      </c>
+      <c r="D238" t="s">
+        <v>487</v>
+      </c>
+      <c r="E238" t="s">
+        <v>726</v>
+      </c>
+      <c r="F238">
+        <v>57</v>
+      </c>
+      <c r="G238">
+        <v>2</v>
+      </c>
+      <c r="H238" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>8</v>
+      </c>
+      <c r="B239">
+        <v>46</v>
+      </c>
+      <c r="C239" t="s">
+        <v>249</v>
+      </c>
+      <c r="D239" t="s">
+        <v>488</v>
+      </c>
+      <c r="E239" t="s">
+        <v>727</v>
+      </c>
+      <c r="F239">
+        <v>22</v>
+      </c>
+      <c r="G239">
+        <v>3</v>
+      </c>
+      <c r="H239" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>8</v>
+      </c>
+      <c r="B240">
+        <v>46</v>
+      </c>
+      <c r="C240" t="s">
+        <v>250</v>
+      </c>
+      <c r="D240" t="s">
+        <v>489</v>
+      </c>
+      <c r="E240" t="s">
+        <v>728</v>
+      </c>
+      <c r="F240">
+        <v>22</v>
+      </c>
+      <c r="G240">
+        <v>3</v>
+      </c>
+      <c r="H240" t="s">
+        <v>913</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor The masking experiment analysis code and make it much more general
</commit_message>
<xml_diff>
--- a/Exp_Record_Alfa.xlsx
+++ b/Exp_Record_Alfa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B128A9-B208-4697-B419-508C4BEF5CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA33BE30-32EB-4C28-88AB-D55E62B5D1DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7252,11 +7252,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A423" workbookViewId="0">
-      <selection activeCell="L441" sqref="L441"/>
+    <sheetView tabSelected="1" topLeftCell="A402" workbookViewId="0">
+      <selection activeCell="N412" sqref="N412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -16220,6 +16223,9 @@
       <c r="G418">
         <v>26</v>
       </c>
+      <c r="H418">
+        <v>3</v>
+      </c>
       <c r="I418" t="s">
         <v>1678</v>
       </c>
@@ -16240,6 +16246,9 @@
       <c r="G419">
         <v>9</v>
       </c>
+      <c r="H419">
+        <v>4</v>
+      </c>
       <c r="I419" t="s">
         <v>1679</v>
       </c>
@@ -16280,6 +16289,9 @@
       <c r="G421">
         <v>9</v>
       </c>
+      <c r="H421">
+        <v>4</v>
+      </c>
       <c r="I421" t="s">
         <v>1681</v>
       </c>
@@ -16300,6 +16312,9 @@
       <c r="G422">
         <v>9</v>
       </c>
+      <c r="H422">
+        <v>4</v>
+      </c>
       <c r="I422" t="s">
         <v>1682</v>
       </c>
@@ -16320,6 +16335,9 @@
       <c r="G423">
         <v>9</v>
       </c>
+      <c r="H423">
+        <v>4</v>
+      </c>
       <c r="I423" t="s">
         <v>1682</v>
       </c>
@@ -16340,6 +16358,9 @@
       <c r="G424">
         <v>9</v>
       </c>
+      <c r="H424">
+        <v>4</v>
+      </c>
       <c r="I424" t="s">
         <v>1682</v>
       </c>
@@ -16359,6 +16380,9 @@
       </c>
       <c r="G425">
         <v>9</v>
+      </c>
+      <c r="H425">
+        <v>4</v>
       </c>
       <c r="I425" t="s">
         <v>1683</v>

</xml_diff>